<commit_message>
added the excel section in batches and manages the batches from training program
</commit_message>
<xml_diff>
--- a/public/Enrollment_Sample.xlsx
+++ b/public/Enrollment_Sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>fullName</t>
   </si>
@@ -25,9 +25,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>coursesInterested</t>
-  </si>
-  <si>
     <t>designation</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>rahul@gmail.com</t>
   </si>
   <si>
-    <t>C++ Programming</t>
-  </si>
-  <si>
     <t>Student</t>
   </si>
   <si>
@@ -59,9 +53,6 @@
   </si>
   <si>
     <t>sneha@gmail.com</t>
-  </si>
-  <si>
-    <t>React.js Mastery Course</t>
   </si>
   <si>
     <t>Intern</t>
@@ -414,7 +405,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -423,9 +414,8 @@
     <col min="1" max="1" style="2" width="13.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="10.862142857142858" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="2" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="37.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="13.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -444,48 +434,39 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>